<commit_message>
Updated Patient Database and Patient ClinicianPlot
Updated Patient Database and Patient ClinicianPlot
</commit_message>
<xml_diff>
--- a/20141213_DataBasePrototype.xlsx
+++ b/20141213_DataBasePrototype.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Neural Engineering Laboraroty</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>15, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Experiment, Device serial, Device location(s), </t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -240,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,11 +544,12 @@
     <col min="3" max="3" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
-    <col min="7" max="9" width="35.5703125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="35.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -573,8 +577,11 @@
       <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -603,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
@@ -630,7 +637,7 @@
       </c>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -641,7 +648,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -652,7 +659,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -663,7 +670,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -674,7 +681,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -685,7 +692,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -696,7 +703,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -707,7 +714,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -718,7 +725,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
     </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -729,7 +736,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -740,7 +747,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -751,7 +758,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -762,7 +769,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>

</xml_diff>